<commit_message>
TCL01 scripts in test suite
</commit_message>
<xml_diff>
--- a/InputFiles/TC07_Canine_StudyTCL01-SampSite_FileTyp_FileForm.xlsx
+++ b/InputFiles/TC07_Canine_StudyTCL01-SampSite_FileTyp_FileForm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DC897B-05A5-4739-B2CB-E55F8F6007C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91885B75-5E89-4398-A61D-4A008494F251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>WebExcel</t>
   </si>
@@ -63,31 +63,10 @@
     <t>cartQuery</t>
   </si>
   <si>
-    <t>TC01_Canine_StudyTCL01-Diag_PrimDisSite_Breed_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC01_Canine_StudyTCL01-Diag_PrimDisSite_Breed_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-MATCH (c)&lt;--(diag:diagnosis)
- WHERE s.clinical_study_designation IN ['TCL01'] and  diag.disease_term in ['Bladder Cancer'] and diag.primary_disease_site in ['Bladder'] and demo.breed in ['Mixed Breed']
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
-RETURN  
-       coalesce(c.case_id, '') AS `Case ID`,
-       coalesce(s.clinical_study_designation, '') AS `Study Code`,
-       coalesce(s.clinical_study_type, '') AS  `Study Type`,
-       coalesce(demo.breed, '') AS Breed ,
-       coalesce(diag.disease_term, '') AS Diagnosis ,
-       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
-       coalesce(CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END, '') AS Age,
-       coalesce(demo.sex, '') AS Sex,
-       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
-       coalesce(diag.best_response, '') AS `Response to Treatment`,
-       coalesce(co.cohort_description, '') AS `Cohort`</t>
+    <t>TC07_Canine_StudyTCL01-SampSite_FileTyp_FileForm_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC07_Canine_StudyTCL01-SampSite_FileTyp_FileForm_Breed_WebData.xlsx</t>
   </si>
   <si>
     <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
@@ -96,7 +75,7 @@
 OPTIONAL MATCH (f:file)-[*]-&gt;(c)
 OPTIONAL MATCH (sf:file)--&gt;(s)
 WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
-WHERE s.clinical_study_designation IN ['TCL01'] and  diag.disease_term in ['Bladder Cancer'] and diag.primary_disease_site in ['Bladder'] and demo.breed in ['Mixed Breed']
+WHERE s.clinical_study_designation IN ['TCL01'] and  diag.disease_term in ['Bladder Cancer'] and samp.sample_site in ['Bladder'] and demo.breed in ['Mixed Breed'] 
 RETURN  
     count(distinct p) AS Programs,
     count(distinct s) AS Studies,
@@ -112,7 +91,7 @@
 OPTIONAL MATCH (f:file)-[*]-&gt;(c)
 OPTIONAL MATCH (sf:file)--&gt;(s)
 WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
-WHERE s.clinical_study_designation IN ['TCL01'] and  diag.disease_term in ['Bladder Cancer'] and diag.primary_disease_site in ['Bladder'] and demo.breed in ['Mixed Breed']]
+WHERE s.clinical_study_designation IN ['TCL01'] and  diag.disease_term in ['Bladder Cancer'] and samp.sample_site in ['Bladder'] and demo.breed in ['Mixed Breed']
 RETURN  
     count(distinct p) AS Programs,
     count(distinct s) AS Studies,
@@ -124,8 +103,8 @@
   <si>
     <t xml:space="preserve">  MATCH (f:file)--&gt;(s:study)
 MATCH (s)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
- WHERE s.clinical_study_designation IN ['TCL01'] and  diag.disease_term in ['Bladder Cancer'] and diag.primary_disease_site in ['Bladder'] and demo.breed in ['Mixed Breed']
-WITH DISTINCT f,  s, c, demo, diag
+WHERE s.clinical_study_designation IN ['TCL01'] and  diag.disease_term in ['Bladder Cancer'] and samp.sample_site in ['Bladder'] and demo.breed in ['Mixed Breed'] 
+ WITH DISTINCT f,  s, c, demo, diag
 WITH
         f, c, demo, diag, s,
         ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
@@ -148,12 +127,53 @@
   coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
   </si>
   <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+MATCH (samp:sample)--&gt;(c)
+MATCH (c)&lt;--(diag:diagnosis)
+WHERE s.clinical_study_designation IN ['TCL01'] and  diag.disease_term in ['Bladder Cancer'] and samp.sample_site in ['Bladder'] and demo.breed in ['Mixed Breed']   
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  
+       coalesce(c.case_id, '') AS `Case ID`,
+       coalesce(s.clinical_study_designation, '') AS `Study Code`,
+       coalesce(s.clinical_study_type, '') AS  `Study Type`,
+       coalesce(demo.breed, '') AS Breed ,
+       coalesce(diag.disease_term, '') AS Diagnosis ,
+       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
+       coalesce(CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END, '') AS Age,
+       coalesce(demo.sex, '') AS Sex,
+       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+       coalesce(diag.best_response, '') AS `Response to Treatment`,
+       coalesce(co.cohort_description, '') AS `Cohort`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+WHERE s.clinical_study_designation IN ['TCL01'] and samp.sample_site in ['Bone'] and f.file_type in ['Index File'] and f.file_format in ['Bai']  
+WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(demo.breed,'') AS Breed,
+        coalesce(diag.disease_term,'') AS Diagnosis, 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
+  </si>
+  <si>
     <t>MATCH (f:file)--&gt;(parent)
 WITH DISTINCT f, parent
+MATCH (s:study)
 MATCH (diag:diagnosis)--&gt;(c)
 OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
 MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
-WHERE s.clinical_study_designation IN ['TCL01'] and  diag.disease_term in ['Bladder Cancer'] and diag.primary_disease_site in ['Bladder'] and demo.breed in ['Mixed Breed']
+WHERE s.clinical_study_designation IN ['TCL01'] and samp.sample_site in ['Bone'] and f.file_type in ['Index File'] and f.file_format in ['bai']  
 OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp)
 WITH
         f, parent, c, demo, diag, s, samp,
@@ -181,21 +201,20 @@
         coalesce(diag.disease_term,'') AS Diagnosis</t>
   </si>
   <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
-WHERE s.clinical_study_designation IN ['TCL01'] and  diag.disease_term in ['Bladder Cancer'] and diag.primary_disease_site in ['Bladder'] and demo.breed in ['Mixed Breed']
-WITH DISTINCT samp AS samp, c, demo, diag
-RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed,
-        coalesce(diag.disease_term,'') AS Diagnosis, 
-        coalesce(samp.sample_site, '') AS `Sample Site`,
-        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
-        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
-        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
-        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
-        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
-        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
-        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+WHERE s.clinical_study_designation IN ['TCL01'] and samp.sample_site in ['Bone'] and f.file_type in ['Index File'] and f.file_format in ['bai']  
+RETURN  
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
   </si>
 </sst>
 </file>
@@ -567,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +600,7 @@
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -606,13 +625,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>10</v>
@@ -626,13 +645,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
@@ -646,13 +665,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
@@ -666,13 +685,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
commit before backup aug 23
</commit_message>
<xml_diff>
--- a/InputFiles/TC07_Canine_StudyTCL01-SampSite_FileTyp_FileForm.xlsx
+++ b/InputFiles/TC07_Canine_StudyTCL01-SampSite_FileTyp_FileForm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91885B75-5E89-4398-A61D-4A008494F251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83B8F40-8D77-408C-86CA-C114296EC117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -75,22 +75,6 @@
 OPTIONAL MATCH (f:file)-[*]-&gt;(c)
 OPTIONAL MATCH (sf:file)--&gt;(s)
 WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
-WHERE s.clinical_study_designation IN ['TCL01'] and  diag.disease_term in ['Bladder Cancer'] and samp.sample_site in ['Bladder'] and demo.breed in ['Mixed Breed'] 
-RETURN  
-    count(distinct p) AS Programs,
-    count(distinct s) AS Studies,
-    count(distinct c) AS Cases,
-    count(distinct samp) AS Samples,
-    count(distinct f) AS `Case Files`,
-    count(distinct sf) AS `Study Files`</t>
-  </si>
-  <si>
-    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
-OPTIONAL MATCH (f:file)-[*]-&gt;(c)
-OPTIONAL MATCH (sf:file)--&gt;(s)
-WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
 WHERE s.clinical_study_designation IN ['TCL01'] and  diag.disease_term in ['Bladder Cancer'] and samp.sample_site in ['Bladder'] and demo.breed in ['Mixed Breed']
 RETURN  
     count(distinct p) AS Programs,
@@ -101,58 +85,75 @@
     count(distinct sf) AS `Study Files`</t>
   </si>
   <si>
-    <t xml:space="preserve">  MATCH (f:file)--&gt;(s:study)
-MATCH (s)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['TCL01'] and  diag.disease_term in ['Bladder Cancer'] and samp.sample_site in ['Bladder'] and demo.breed in ['Mixed Breed'] 
- WITH DISTINCT f,  s, c, demo, diag
-WITH
-        f, c, demo, diag, s,
-        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
-        toInteger(floor(log(f.file_size)/log(1024))) as i,
-        2 as precision
-WITH    
-        f, c, demo, diag, s,
-        f.file_size /(1024^i) AS value, 10^precision AS factor,
-        units[i] as unit
-        WITH    
-        f,  c, demo, diag, s, unit,
-        round(factor * value)/factor AS size
-RETURN DISTINCT
-  coalesce(f.file_name, '') AS `File Name`,
-  coalesce(f.file_type, '') AS `File Type`,
-  coalesce("study", '') AS `Association`,
-  coalesce(f.file_description, '') AS `Description`,
-  coalesce(f.file_format, '') AS  Format,
-  CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
-  coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+WHERE s.clinical_study_designation IN ['TCL01'] and samp.sample_site in ['Bone'] and f.file_type in ['Index File'] and f.file_format in ['bai']  
+RETURN  
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;--(c:case)
+WHERE s.clinical_study_designation IN ['TCL01']
 MATCH (samp:sample)--&gt;(c)
+WHERE samp.sample_site in ['Bone']
+MATCH (f:file)-[*]-&gt;(c)
+WHERE f.file_type in ['Index File'] AND f.file_format in ['bai']
 MATCH (c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['TCL01'] and  diag.disease_term in ['Bladder Cancer'] and samp.sample_site in ['Bladder'] and demo.breed in ['Mixed Breed']   
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+MATCH (c)&lt;--(demo:demographic)
+OPTIONAL MATCH (co:cohort)&lt;--(c)
+WITH DISTINCT c, s, demo, diag, f, samp, co, 
+    demo.patient_age_at_enrollment AS age, 
+    demo.weight as weight
+RETURN
+    coalesce(c.case_id, '') AS `Case ID`,
+    coalesce(s.clinical_study_designation, '') AS `Study Code`,
+    coalesce(s.clinical_study_type, '') AS  `Study Type`,
+    coalesce(demo.breed, '') AS Breed ,
+    coalesce(diag.disease_term, '') AS Diagnosis ,
+    coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
+    coalesce(CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END, '') AS Age,
+    coalesce(demo.sex, '') AS Sex,
+    coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+    coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+    coalesce(diag.best_response, '') AS `Response to Treatment`,
+    coalesce(co.cohort_description, '') AS `Cohort`</t>
+  </si>
+  <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+MATCH (s:study)&lt;--(c:case)
+WHERE s.clinical_study_designation IN ['TCL01']
+MATCH (samp:sample)--&gt;(c)
+WHERE samp.sample_site in ['Bone']
+MATCH (c)&lt;--(diag:diagnosis)
+MATCH (c)&lt;--(demo:demographic)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+MATCH (f:file)-[*]-&gt;(c)
+WHERE f.file_type in ['Index File'] AND f.file_format in ['bai']
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT c, s, demo, diag, f, samp,p, sf
 RETURN  
-       coalesce(c.case_id, '') AS `Case ID`,
-       coalesce(s.clinical_study_designation, '') AS `Study Code`,
-       coalesce(s.clinical_study_type, '') AS  `Study Type`,
-       coalesce(demo.breed, '') AS Breed ,
-       coalesce(diag.disease_term, '') AS Diagnosis ,
-       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
-       coalesce(CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END, '') AS Age,
-       coalesce(demo.sex, '') AS Sex,
-       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
-       coalesce(diag.best_response, '') AS `Response to Treatment`,
-       coalesce(co.cohort_description, '') AS `Cohort`</t>
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
   </si>
   <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
-MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-WHERE s.clinical_study_designation IN ['TCL01'] and samp.sample_site in ['Bone'] and f.file_type in ['Index File'] and f.file_format in ['Bai']  
-WITH DISTINCT samp AS samp, c, demo, diag
+WHERE s.clinical_study_designation IN ['TCL01'] and samp.sample_site in ['Bone']
+MATCH (f:file)-[*]-&gt;(c)
+WHERE f.file_type in ['Index File'] AND f.file_format in ['bai']
+WITH DISTINCT samp AS samp, c, s, demo, diag
 RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
         coalesce(c.case_id, '') AS `Case ID`, 
         coalesce(demo.breed,'') AS Breed,
@@ -169,12 +170,11 @@
   <si>
     <t>MATCH (f:file)--&gt;(parent)
 WITH DISTINCT f, parent
-MATCH (s:study)
+MATCH (f:file)-[*]-&gt;(c) WHERE f.file_type in ['Index File'] AND f.file_format in ['bai']
+MATCH (s:study)&lt;--(c:case) WHERE s.clinical_study_designation IN ['TCL01']
+MATCH (samp:sample)--&gt;(c) WHERE samp.sample_site in ['Bone']
 MATCH (diag:diagnosis)--&gt;(c)
-OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
-WHERE s.clinical_study_designation IN ['TCL01'] and samp.sample_site in ['Bone'] and f.file_type in ['Index File'] and f.file_format in ['bai']  
-OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp)
+MATCH (c)&lt;--(demo:demographic)
 WITH
         f, parent, c, demo, diag, s, samp,
         ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
@@ -201,20 +201,30 @@
         coalesce(diag.disease_term,'') AS Diagnosis</t>
   </si>
   <si>
-    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
-OPTIONAL MATCH (f:file)-[*]-&gt;(c)
-OPTIONAL MATCH (sf:file)--&gt;(s)
-WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
-WHERE s.clinical_study_designation IN ['TCL01'] and samp.sample_site in ['Bone'] and f.file_type in ['Index File'] and f.file_format in ['bai']  
-RETURN  
-    count(distinct p) AS Programs,
-    count(distinct s) AS Studies,
-    count(distinct c) AS Cases,
-    count(distinct samp) AS Samples,
-    count(distinct f) AS `Case Files`,
-    count(distinct sf) AS `Study Files`</t>
+    <t>MATCH (s:study)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
+  WHERE s.clinical_study_designation IN ['TCL01']
+MATCH (samp:sample)--&gt;(c) WHERE samp.sample_site in ['Bone']
+MATCH (f:file)-[:of_study]-&gt;(s) WHERE f.file_type in ['Index File'] AND f.file_format in ['bai']
+WITH
+        f, c, demo, diag, s,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, c, demo, diag, s,
+        f.file_size /(1024^i) AS value, 10^precision AS factor,
+        units[i] as unit
+        WITH
+        f,  c, demo, diag, s, unit,
+        round(factor * value)/factor AS size
+RETURN DISTINCT
+  coalesce(f.file_name, '') AS `File Name`,
+  coalesce(f.file_type, '') AS `File Type`,
+  coalesce("study", '') AS `Association`,
+  coalesce(f.file_description, '') AS `Description`,
+  coalesce(f.file_format, '') AS  Format,
+  CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+  coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
   </si>
 </sst>
 </file>
@@ -586,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,13 +635,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>10</v>
@@ -640,7 +650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="375" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="390" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -648,10 +658,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
@@ -668,10 +678,10 @@
         <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
@@ -685,13 +695,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
ICDC QA obj and profile - commit from Maryland
</commit_message>
<xml_diff>
--- a/InputFiles/TC07_Canine_StudyTCL01-SampSite_FileTyp_FileForm.xlsx
+++ b/InputFiles/TC07_Canine_StudyTCL01-SampSite_FileTyp_FileForm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91885B75-5E89-4398-A61D-4A008494F251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83B8F40-8D77-408C-86CA-C114296EC117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -75,22 +75,6 @@
 OPTIONAL MATCH (f:file)-[*]-&gt;(c)
 OPTIONAL MATCH (sf:file)--&gt;(s)
 WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
-WHERE s.clinical_study_designation IN ['TCL01'] and  diag.disease_term in ['Bladder Cancer'] and samp.sample_site in ['Bladder'] and demo.breed in ['Mixed Breed'] 
-RETURN  
-    count(distinct p) AS Programs,
-    count(distinct s) AS Studies,
-    count(distinct c) AS Cases,
-    count(distinct samp) AS Samples,
-    count(distinct f) AS `Case Files`,
-    count(distinct sf) AS `Study Files`</t>
-  </si>
-  <si>
-    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
-OPTIONAL MATCH (f:file)-[*]-&gt;(c)
-OPTIONAL MATCH (sf:file)--&gt;(s)
-WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
 WHERE s.clinical_study_designation IN ['TCL01'] and  diag.disease_term in ['Bladder Cancer'] and samp.sample_site in ['Bladder'] and demo.breed in ['Mixed Breed']
 RETURN  
     count(distinct p) AS Programs,
@@ -101,58 +85,75 @@
     count(distinct sf) AS `Study Files`</t>
   </si>
   <si>
-    <t xml:space="preserve">  MATCH (f:file)--&gt;(s:study)
-MATCH (s)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['TCL01'] and  diag.disease_term in ['Bladder Cancer'] and samp.sample_site in ['Bladder'] and demo.breed in ['Mixed Breed'] 
- WITH DISTINCT f,  s, c, demo, diag
-WITH
-        f, c, demo, diag, s,
-        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
-        toInteger(floor(log(f.file_size)/log(1024))) as i,
-        2 as precision
-WITH    
-        f, c, demo, diag, s,
-        f.file_size /(1024^i) AS value, 10^precision AS factor,
-        units[i] as unit
-        WITH    
-        f,  c, demo, diag, s, unit,
-        round(factor * value)/factor AS size
-RETURN DISTINCT
-  coalesce(f.file_name, '') AS `File Name`,
-  coalesce(f.file_type, '') AS `File Type`,
-  coalesce("study", '') AS `Association`,
-  coalesce(f.file_description, '') AS `Description`,
-  coalesce(f.file_format, '') AS  Format,
-  CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
-  coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+WHERE s.clinical_study_designation IN ['TCL01'] and samp.sample_site in ['Bone'] and f.file_type in ['Index File'] and f.file_format in ['bai']  
+RETURN  
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;--(c:case)
+WHERE s.clinical_study_designation IN ['TCL01']
 MATCH (samp:sample)--&gt;(c)
+WHERE samp.sample_site in ['Bone']
+MATCH (f:file)-[*]-&gt;(c)
+WHERE f.file_type in ['Index File'] AND f.file_format in ['bai']
 MATCH (c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['TCL01'] and  diag.disease_term in ['Bladder Cancer'] and samp.sample_site in ['Bladder'] and demo.breed in ['Mixed Breed']   
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+MATCH (c)&lt;--(demo:demographic)
+OPTIONAL MATCH (co:cohort)&lt;--(c)
+WITH DISTINCT c, s, demo, diag, f, samp, co, 
+    demo.patient_age_at_enrollment AS age, 
+    demo.weight as weight
+RETURN
+    coalesce(c.case_id, '') AS `Case ID`,
+    coalesce(s.clinical_study_designation, '') AS `Study Code`,
+    coalesce(s.clinical_study_type, '') AS  `Study Type`,
+    coalesce(demo.breed, '') AS Breed ,
+    coalesce(diag.disease_term, '') AS Diagnosis ,
+    coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
+    coalesce(CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END, '') AS Age,
+    coalesce(demo.sex, '') AS Sex,
+    coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+    coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+    coalesce(diag.best_response, '') AS `Response to Treatment`,
+    coalesce(co.cohort_description, '') AS `Cohort`</t>
+  </si>
+  <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+MATCH (s:study)&lt;--(c:case)
+WHERE s.clinical_study_designation IN ['TCL01']
+MATCH (samp:sample)--&gt;(c)
+WHERE samp.sample_site in ['Bone']
+MATCH (c)&lt;--(diag:diagnosis)
+MATCH (c)&lt;--(demo:demographic)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+MATCH (f:file)-[*]-&gt;(c)
+WHERE f.file_type in ['Index File'] AND f.file_format in ['bai']
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT c, s, demo, diag, f, samp,p, sf
 RETURN  
-       coalesce(c.case_id, '') AS `Case ID`,
-       coalesce(s.clinical_study_designation, '') AS `Study Code`,
-       coalesce(s.clinical_study_type, '') AS  `Study Type`,
-       coalesce(demo.breed, '') AS Breed ,
-       coalesce(diag.disease_term, '') AS Diagnosis ,
-       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
-       coalesce(CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END, '') AS Age,
-       coalesce(demo.sex, '') AS Sex,
-       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
-       coalesce(diag.best_response, '') AS `Response to Treatment`,
-       coalesce(co.cohort_description, '') AS `Cohort`</t>
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
   </si>
   <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
-MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-WHERE s.clinical_study_designation IN ['TCL01'] and samp.sample_site in ['Bone'] and f.file_type in ['Index File'] and f.file_format in ['Bai']  
-WITH DISTINCT samp AS samp, c, demo, diag
+WHERE s.clinical_study_designation IN ['TCL01'] and samp.sample_site in ['Bone']
+MATCH (f:file)-[*]-&gt;(c)
+WHERE f.file_type in ['Index File'] AND f.file_format in ['bai']
+WITH DISTINCT samp AS samp, c, s, demo, diag
 RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
         coalesce(c.case_id, '') AS `Case ID`, 
         coalesce(demo.breed,'') AS Breed,
@@ -169,12 +170,11 @@
   <si>
     <t>MATCH (f:file)--&gt;(parent)
 WITH DISTINCT f, parent
-MATCH (s:study)
+MATCH (f:file)-[*]-&gt;(c) WHERE f.file_type in ['Index File'] AND f.file_format in ['bai']
+MATCH (s:study)&lt;--(c:case) WHERE s.clinical_study_designation IN ['TCL01']
+MATCH (samp:sample)--&gt;(c) WHERE samp.sample_site in ['Bone']
 MATCH (diag:diagnosis)--&gt;(c)
-OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
-WHERE s.clinical_study_designation IN ['TCL01'] and samp.sample_site in ['Bone'] and f.file_type in ['Index File'] and f.file_format in ['bai']  
-OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp)
+MATCH (c)&lt;--(demo:demographic)
 WITH
         f, parent, c, demo, diag, s, samp,
         ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
@@ -201,20 +201,30 @@
         coalesce(diag.disease_term,'') AS Diagnosis</t>
   </si>
   <si>
-    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
-OPTIONAL MATCH (f:file)-[*]-&gt;(c)
-OPTIONAL MATCH (sf:file)--&gt;(s)
-WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
-WHERE s.clinical_study_designation IN ['TCL01'] and samp.sample_site in ['Bone'] and f.file_type in ['Index File'] and f.file_format in ['bai']  
-RETURN  
-    count(distinct p) AS Programs,
-    count(distinct s) AS Studies,
-    count(distinct c) AS Cases,
-    count(distinct samp) AS Samples,
-    count(distinct f) AS `Case Files`,
-    count(distinct sf) AS `Study Files`</t>
+    <t>MATCH (s:study)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
+  WHERE s.clinical_study_designation IN ['TCL01']
+MATCH (samp:sample)--&gt;(c) WHERE samp.sample_site in ['Bone']
+MATCH (f:file)-[:of_study]-&gt;(s) WHERE f.file_type in ['Index File'] AND f.file_format in ['bai']
+WITH
+        f, c, demo, diag, s,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, c, demo, diag, s,
+        f.file_size /(1024^i) AS value, 10^precision AS factor,
+        units[i] as unit
+        WITH
+        f,  c, demo, diag, s, unit,
+        round(factor * value)/factor AS size
+RETURN DISTINCT
+  coalesce(f.file_name, '') AS `File Name`,
+  coalesce(f.file_type, '') AS `File Type`,
+  coalesce("study", '') AS `Association`,
+  coalesce(f.file_description, '') AS `Description`,
+  coalesce(f.file_format, '') AS  Format,
+  CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+  coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
   </si>
 </sst>
 </file>
@@ -586,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,13 +635,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>10</v>
@@ -640,7 +650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="375" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="390" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -648,10 +658,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
@@ -668,10 +678,10 @@
         <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
@@ -685,13 +695,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>

</xml_diff>